<commit_message>
Atualiza dados da liga eliminacao
</commit_message>
<xml_diff>
--- a/liga_eliminacao/datasets_liga_eliminacao/Pontuacoes_Por_Rodada_Liga_Eliminacao.xlsx
+++ b/liga_eliminacao/datasets_liga_eliminacao/Pontuacoes_Por_Rodada_Liga_Eliminacao.xlsx
@@ -112,9 +112,6 @@
     <t>cartola scheuer17</t>
   </si>
   <si>
-    <t>BORGES ITAQUI F.C.</t>
-  </si>
-  <si>
     <t>S.E.R. GRILLO</t>
   </si>
   <si>
@@ -149,6 +146,9 @@
   </si>
   <si>
     <t>Grêmio imortal 37</t>
+  </si>
+  <si>
+    <t>Grêmio imortal 36</t>
   </si>
   <si>
     <t>FIGUEIRA DA ILHA</t>
@@ -724,7 +724,7 @@
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="1">
-        <v>3914981</v>
+        <v>5823700</v>
       </c>
       <c r="B13" t="s">
         <v>32</v>
@@ -735,7 +735,7 @@
     </row>
     <row r="14" spans="1:21">
       <c r="A14" s="1">
-        <v>5823700</v>
+        <v>13707047</v>
       </c>
       <c r="B14" t="s">
         <v>33</v>
@@ -746,7 +746,7 @@
     </row>
     <row r="15" spans="1:21">
       <c r="A15" s="1">
-        <v>13707047</v>
+        <v>13913874</v>
       </c>
       <c r="B15" t="s">
         <v>34</v>
@@ -757,7 +757,7 @@
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="1">
-        <v>13913874</v>
+        <v>13951133</v>
       </c>
       <c r="B16" t="s">
         <v>35</v>
@@ -768,7 +768,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="1">
-        <v>13951133</v>
+        <v>14124559</v>
       </c>
       <c r="B17" t="s">
         <v>36</v>
@@ -779,7 +779,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="1">
-        <v>14124559</v>
+        <v>18223508</v>
       </c>
       <c r="B18" t="s">
         <v>37</v>
@@ -790,7 +790,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="1">
-        <v>18223508</v>
+        <v>18344271</v>
       </c>
       <c r="B19" t="s">
         <v>38</v>
@@ -801,7 +801,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="1">
-        <v>18344271</v>
+        <v>18642587</v>
       </c>
       <c r="B20" t="s">
         <v>39</v>
@@ -812,7 +812,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="1">
-        <v>18642587</v>
+        <v>18661583</v>
       </c>
       <c r="B21" t="s">
         <v>40</v>
@@ -823,7 +823,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="1">
-        <v>18661583</v>
+        <v>19033717</v>
       </c>
       <c r="B22" t="s">
         <v>41</v>
@@ -834,7 +834,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="1">
-        <v>19033717</v>
+        <v>20696550</v>
       </c>
       <c r="B23" t="s">
         <v>42</v>
@@ -845,7 +845,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="1">
-        <v>20696550</v>
+        <v>24468241</v>
       </c>
       <c r="B24" t="s">
         <v>43</v>
@@ -856,7 +856,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="1">
-        <v>24468241</v>
+        <v>24856400</v>
       </c>
       <c r="B25" t="s">
         <v>44</v>

</xml_diff>

<commit_message>
Atualiza regras de parcial na Liga Eliminacao
</commit_message>
<xml_diff>
--- a/liga_eliminacao/datasets_liga_eliminacao/Pontuacoes_Por_Rodada_Liga_Eliminacao.xlsx
+++ b/liga_eliminacao/datasets_liga_eliminacao/Pontuacoes_Por_Rodada_Liga_Eliminacao.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>Time</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>Rodada 19</t>
+  </si>
+  <si>
+    <t>Parcial Rodada 1</t>
   </si>
   <si>
     <t>time_id</t>
@@ -530,15 +533,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:U33"/>
+  <dimension ref="A1:V33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:21">
+    <row r="1" spans="1:22">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -600,357 +603,456 @@
       <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:21">
+      <c r="V1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22">
       <c r="A2" s="1">
         <v>117598</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:21">
+      <c r="V2">
+        <v>59.56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
       <c r="A3" s="1">
         <v>186283</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:21">
+      <c r="V3">
+        <v>45.46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
       <c r="A4" s="1">
         <v>212042</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:21">
+      <c r="V4">
+        <v>64.95999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22">
       <c r="A5" s="1">
         <v>335716</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:21">
+      <c r="V5">
+        <v>61.8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
       <c r="A6" s="1">
         <v>479510</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:21">
+      <c r="V6">
+        <v>50.76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7" s="1">
         <v>528730</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:21">
+      <c r="V7">
+        <v>56.65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
       <c r="A8" s="1">
         <v>1273719</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:21">
+      <c r="V8">
+        <v>59.86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
       <c r="A9" s="1">
         <v>1747619</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:21">
+      <c r="V9">
+        <v>39.66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
       <c r="A10" s="1">
         <v>3447341</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:21">
+      <c r="V10">
+        <v>60.66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22">
       <c r="A11" s="1">
         <v>3708025</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:21">
+      <c r="V11">
+        <v>23.26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22">
       <c r="A12" s="1">
         <v>3851966</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:21">
+      <c r="V12">
+        <v>53.06</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22">
       <c r="A13" s="1">
         <v>5823700</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:21">
+      <c r="V13">
+        <v>59.76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22">
       <c r="A14" s="1">
         <v>13707047</v>
       </c>
       <c r="B14" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:21">
+      <c r="V14">
+        <v>34.76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22">
       <c r="A15" s="1">
         <v>13913874</v>
       </c>
       <c r="B15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:21">
+      <c r="V15">
+        <v>69.56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
       <c r="A16" s="1">
         <v>13951133</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="V16">
+        <v>41.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22">
       <c r="A17" s="1">
         <v>14124559</v>
       </c>
       <c r="B17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="V17">
+        <v>73.66</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22">
       <c r="A18" s="1">
         <v>18223508</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="V18">
+        <v>51.05</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22">
       <c r="A19" s="1">
         <v>18344271</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="V19">
+        <v>49.16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:22">
       <c r="A20" s="1">
         <v>18642587</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="V20">
+        <v>50.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22">
       <c r="A21" s="1">
         <v>18661583</v>
       </c>
       <c r="B21" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="V21">
+        <v>44.46</v>
+      </c>
+    </row>
+    <row r="22" spans="1:22">
       <c r="A22" s="1">
         <v>19033717</v>
       </c>
       <c r="B22" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="V22">
+        <v>69.76000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22">
       <c r="A23" s="1">
         <v>20696550</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="V23">
+        <v>58.4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22">
       <c r="A24" s="1">
         <v>24468241</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="V24">
+        <v>43.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22">
       <c r="A25" s="1">
         <v>24856400</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="V25">
+        <v>30.6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22">
       <c r="A26" s="1">
         <v>25565675</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="V26">
+        <v>44.06</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22">
       <c r="A27" s="1">
         <v>25811332</v>
       </c>
       <c r="B27" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C27">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="V27">
+        <v>38.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22">
       <c r="A28" s="1">
         <v>28741323</v>
       </c>
       <c r="B28" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="V28">
+        <v>57.76</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22">
       <c r="A29" s="1">
         <v>29228373</v>
       </c>
       <c r="B29" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="V29">
+        <v>34.36</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22">
       <c r="A30" s="1">
         <v>44810918</v>
       </c>
       <c r="B30" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="V30">
+        <v>54.36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22">
       <c r="A31" s="1">
         <v>47544767</v>
       </c>
       <c r="B31" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:3">
+      <c r="V31">
+        <v>69.26000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22">
       <c r="A32" s="1">
         <v>48498051</v>
       </c>
       <c r="B32" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:3">
+      <c r="V32">
+        <v>60.36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22">
       <c r="A33" s="1">
         <v>51010813</v>
       </c>
       <c r="B33" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C33">
         <v>0</v>
+      </c>
+      <c r="V33">
+        <v>39.66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>